<commit_message>
Updated upto 55 TC
</commit_message>
<xml_diff>
--- a/src/main/resources/WebStaff TC ExcelSheet/Automation Test test cases for WebStaff.xlsx
+++ b/src/main/resources/WebStaff TC ExcelSheet/Automation Test test cases for WebStaff.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2824" uniqueCount="370">
   <si>
     <t>Step#</t>
   </si>
@@ -6527,7 +6527,7 @@
         <v>357</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -6545,7 +6545,7 @@
         <v>357</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H15" s="2"/>
     </row>
@@ -6565,7 +6565,7 @@
         <v>357</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H16" s="2"/>
     </row>
@@ -6585,7 +6585,7 @@
         <v>357</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H17" s="2"/>
     </row>
@@ -6603,7 +6603,7 @@
         <v>357</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H18" s="2"/>
     </row>
@@ -6623,7 +6623,7 @@
         <v>357</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H19" s="2"/>
     </row>
@@ -6641,7 +6641,7 @@
         <v>357</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H20" s="2"/>
     </row>
@@ -6661,7 +6661,7 @@
         <v>357</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H21" s="2"/>
     </row>
@@ -6679,7 +6679,7 @@
         <v>357</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H22" s="2"/>
     </row>
@@ -6699,7 +6699,7 @@
         <v>357</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H23" s="2"/>
     </row>
@@ -6717,7 +6717,7 @@
         <v>357</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H24" s="2"/>
     </row>
@@ -6737,7 +6737,7 @@
         <v>357</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H25" s="2"/>
     </row>
@@ -6757,7 +6757,7 @@
         <v>357</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H26" s="2"/>
     </row>
@@ -6775,7 +6775,7 @@
         <v>357</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H27" s="2"/>
     </row>
@@ -6795,7 +6795,7 @@
         <v>357</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H28" s="2"/>
     </row>
@@ -6815,7 +6815,7 @@
         <v>357</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H29" s="2"/>
     </row>
@@ -6833,7 +6833,7 @@
         <v>357</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H30" s="2"/>
     </row>
@@ -6853,7 +6853,7 @@
         <v>357</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H31" s="2"/>
     </row>
@@ -6871,7 +6871,7 @@
         <v>357</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H32" s="2"/>
     </row>
@@ -6891,7 +6891,7 @@
         <v>357</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H33" s="2"/>
     </row>
@@ -6911,7 +6911,7 @@
         <v>357</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H34" s="2"/>
     </row>
@@ -6931,7 +6931,7 @@
         <v>357</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H35" s="2"/>
     </row>
@@ -6949,7 +6949,7 @@
         <v>357</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H36" s="2"/>
     </row>
@@ -6967,7 +6967,7 @@
         <v>357</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H37" s="2"/>
     </row>
@@ -6987,7 +6987,7 @@
         <v>357</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H38" s="2"/>
     </row>
@@ -7005,7 +7005,7 @@
         <v>357</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H39" s="2"/>
     </row>
@@ -7021,8 +7021,12 @@
       <c r="E40" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
+      <c r="F40" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="H40" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -7037,8 +7041,12 @@
       <c r="E41" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
+      <c r="F41" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="H41" s="2"/>
     </row>
     <row customHeight="1" ht="46.5" r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -7051,8 +7059,12 @@
       <c r="E42" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="F42" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="H42" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -7067,8 +7079,12 @@
       <c r="E43" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
+      <c r="F43" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="H43" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -7081,8 +7097,12 @@
       <c r="E44" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
+      <c r="F44" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="H44" s="2"/>
     </row>
     <row customHeight="1" ht="36.75" r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -7095,8 +7115,12 @@
       <c r="E45" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
+      <c r="F45" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="H45" s="2"/>
     </row>
     <row customHeight="1" ht="39" r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -7111,8 +7135,12 @@
       <c r="E46" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
+      <c r="F46" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="H46" s="2"/>
     </row>
     <row customHeight="1" ht="66" r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -7125,8 +7153,12 @@
       <c r="E47" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
+      <c r="F47" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="H47" s="2"/>
     </row>
     <row customHeight="1" ht="34.5" r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -7141,8 +7173,12 @@
       <c r="E48" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
+      <c r="F48" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="H48" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -7157,8 +7193,12 @@
       <c r="E49" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
+      <c r="F49" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="H49" s="2"/>
     </row>
     <row customHeight="1" ht="57" r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -7171,8 +7211,12 @@
       <c r="E50" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
+      <c r="F50" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="H50" s="2"/>
     </row>
     <row customHeight="1" ht="54" r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -7185,8 +7229,12 @@
       <c r="E51" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
+      <c r="F51" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="H51" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -7199,8 +7247,12 @@
       <c r="E52" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
+      <c r="F52" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="H52" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -7215,8 +7267,12 @@
       <c r="E53" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
+      <c r="F53" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="H53" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="54" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Test cases uptaded up to 77
</commit_message>
<xml_diff>
--- a/src/main/resources/WebStaff TC ExcelSheet/Automation Test test cases for WebStaff.xlsx
+++ b/src/main/resources/WebStaff TC ExcelSheet/Automation Test test cases for WebStaff.xlsx
@@ -1,19 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kulandasamyc\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr documentId="13_ncr:1_{BCE85B65-1DF4-4966-831E-BEE955238551}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="7755" windowWidth="20400" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" windowHeight="7725" windowWidth="20400" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="WebStaff_TestCases" r:id="rId1" sheetId="1"/>
     <sheet name="WebStaff_TC" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2824" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1700" uniqueCount="368">
   <si>
     <t>Step#</t>
   </si>
@@ -665,9 +670,6 @@
     <t>System should show 'Find &amp; Import Registrant' modal window.</t>
   </si>
   <si>
-    <t>Based on search, system should filter the registrant with 'Select' link.</t>
-  </si>
-  <si>
     <t>1. Click on 'Select' button.
 2. Click on 'Yes Continue' link on Confirmation window.</t>
   </si>
@@ -752,12 +754,6 @@
     <t>System should take to Find Rooms page and display Hotel Search related fields.</t>
   </si>
   <si>
-    <t>Click on 'View Inventory' link.</t>
-  </si>
-  <si>
-    <t>System should show all Hotels Inventory details.</t>
-  </si>
-  <si>
     <t>Based Arrival and Departure dates, Hotel result should display list of Hotels.</t>
   </si>
   <si>
@@ -789,9 +785,6 @@
   </si>
   <si>
     <t>Lead Occupant</t>
-  </si>
-  <si>
-    <t>Add another occupant and Save.</t>
   </si>
   <si>
     <t>Enter mandatory fields and Save as Lead Occupant.</t>
@@ -814,10 +807,6 @@
     <t>Click on Change Rooms tab.</t>
   </si>
   <si>
-    <t>1. Click on Changes Dates tab..
-2. Without changing Dates, click on Save Changes.</t>
-  </si>
-  <si>
     <t>Change Room modal window should display and show available rooms with 'Select' link.</t>
   </si>
   <si>
@@ -852,15 +841,6 @@
     <t>Release Room</t>
   </si>
   <si>
-    <t>Release Room tab should display.</t>
-  </si>
-  <si>
-    <t>Open Hotel Held state room accordion.</t>
-  </si>
-  <si>
-    <t>Click on 'Release Room' link.</t>
-  </si>
-  <si>
     <t>Hotel CONF#</t>
   </si>
   <si>
@@ -871,44 +851,10 @@
     <t>System should show success message as 'Hotel Confirmation Number: successfully updated.' and entered number should be updated in the field.</t>
   </si>
   <si>
-    <t>1.  Click on edit icon in Nights.
-2. Change Departure Date and Click  on Save Changes.</t>
-  </si>
-  <si>
-    <t>Night</t>
-  </si>
-  <si>
-    <t>Rate</t>
-  </si>
-  <si>
-    <t>1. Click on Rate edit icon.
-2.  Enter 'galaxy' password.
-3. Select rate plan Radio button and Save.</t>
-  </si>
-  <si>
     <t>Selected Rate should update in the Occupant details page and show success message</t>
   </si>
   <si>
     <t>Deposit</t>
-  </si>
-  <si>
-    <t>Click on Deposit edit icon.</t>
-  </si>
-  <si>
-    <t>Edit deposit window should open.</t>
-  </si>
-  <si>
-    <t>Enter Deposit Amount and Save.</t>
-  </si>
-  <si>
-    <t>Rewards</t>
-  </si>
-  <si>
-    <t>1. Click on Rewards edit icon.
-2. Enter Rewards number and Save.</t>
-  </si>
-  <si>
-    <t>Rewards Number should update under the Label.</t>
   </si>
   <si>
     <t>Special Requests.</t>
@@ -1056,10 +1002,6 @@
     <t>System should show success message as 'Room has been successfully released.' and the hotel should remove from the list.</t>
   </si>
   <si>
-    <t>If Room is available it should show message as 'The room is available' and Number of nights should update.
-If room is NOT available it should show message as 'The requested change is not available.' and number Night should show same.</t>
-  </si>
-  <si>
     <t>Deposit label should change to 'Manual' and update the amount.</t>
   </si>
   <si>
@@ -1151,10 +1093,6 @@
     <t>Group Assignment</t>
   </si>
   <si>
-    <t>1. Under Group Assignment.
-2. Click on Select dropdown.</t>
-  </si>
-  <si>
     <t>System should open and show Registrant Group Assigment modal window.</t>
   </si>
   <si>
@@ -1182,9 +1120,6 @@
 3. Click on Save.</t>
   </si>
   <si>
-    <t>Edit FN &amp; LN and click on Save on bottom of the page.</t>
-  </si>
-  <si>
     <t>Add Exhibitor company in SHowMan.</t>
   </si>
   <si>
@@ -1235,6 +1170,71 @@
   </si>
   <si>
     <t>System should NOT show 'CANCELLED' text.</t>
+  </si>
+  <si>
+    <t>Based on search, system should filter the registrant and show with 'Select' link.</t>
+  </si>
+  <si>
+    <t>1. Click on 'View Inventory' link.
+2. Close the Inventory window.</t>
+  </si>
+  <si>
+    <t>System should show all Hotels Inventory details and return back to Hotel Search page after close.</t>
+  </si>
+  <si>
+    <t>Add another occupant by Selecting from the list and Save.</t>
+  </si>
+  <si>
+    <t>Change Lead</t>
+  </si>
+  <si>
+    <t>1. Click on Occupant radio button.
+2. Click Yes.</t>
+  </si>
+  <si>
+    <t>System should change Lead Occupant and confirm with message.</t>
+  </si>
+  <si>
+    <t>Edit Occupant</t>
+  </si>
+  <si>
+    <t>1. Click on edit icon.
+2. Change First Name and click Save.</t>
+  </si>
+  <si>
+    <t>Updated name should display in Occupant page.</t>
+  </si>
+  <si>
+    <t>Delete Occpuant.</t>
+  </si>
+  <si>
+    <t>Click on Delete  Occupant 'x' link.</t>
+  </si>
+  <si>
+    <t>System should show warining message as ' Cannot delete this lead occupant. There are no other occupants in this reservation to assume the lead role' message.</t>
+  </si>
+  <si>
+    <t>1. Click on Change Dates tab..
+2. Without changing Dates, click on Save Changes.</t>
+  </si>
+  <si>
+    <t>Click on 'Send Email' link.</t>
+  </si>
+  <si>
+    <t>System should display ' Confirmation Letter has been sent'.</t>
+  </si>
+  <si>
+    <t>1. Click on Summary Tab. 
+2. Under Group Assignment.
+3. Click on Select dropdown.</t>
+  </si>
+  <si>
+    <t>1. Open Hotel Held state room accordion.
+2. Click on 'Release Room' link.</t>
+  </si>
+  <si>
+    <t>1. Click on Deposit edit icon.
+2. Enter Deposit Amount and Save.</t>
   </si>
   <si>
     <t>Fail</t>
@@ -1243,7 +1243,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1356,7 +1356,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -1715,12 +1715,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J380"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScaleNormal="100">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A35" ySplit="1"/>
-      <selection activeCell="C7" pane="bottomLeft" sqref="C7"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A62" ySplit="1"/>
+      <selection activeCell="D41" pane="bottomLeft" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6241,18 +6241,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J202"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" customWidth="true" width="11.85546875" collapsed="true"/>
     <col min="3" max="3" customWidth="true" style="3" width="18.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="53.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="56.85546875" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="3" width="73.140625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="13.71484375" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="7.12109375" collapsed="true"/>
@@ -6296,16 +6296,16 @@
         <v>113</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>359</v>
+        <v>338</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>361</v>
+        <v>340</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -6314,16 +6314,16 @@
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8" t="s">
-        <v>360</v>
+        <v>339</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>358</v>
+        <v>337</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -6334,16 +6334,16 @@
         <v>181</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -6358,10 +6358,10 @@
         <v>134</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -6370,16 +6370,16 @@
       <c r="B6" s="2"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>115</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -6394,10 +6394,10 @@
         <v>117</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -6412,10 +6412,10 @@
         <v>119</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -6432,10 +6432,10 @@
         <v>121</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H9" s="2"/>
     </row>
@@ -6450,10 +6450,10 @@
         <v>123</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H10" s="2"/>
     </row>
@@ -6468,10 +6468,10 @@
         <v>125</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H11" s="2"/>
     </row>
@@ -6488,10 +6488,10 @@
         <v>136</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H12" s="2"/>
     </row>
@@ -6506,10 +6506,10 @@
         <v>138</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H13" s="2"/>
     </row>
@@ -6524,10 +6524,10 @@
         <v>139</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -6536,16 +6536,16 @@
       <c r="B15" s="2"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8" t="s">
-        <v>364</v>
+        <v>343</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H15" s="2"/>
     </row>
@@ -6559,13 +6559,13 @@
         <v>176</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H16" s="2"/>
     </row>
@@ -6582,10 +6582,10 @@
         <v>129</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H17" s="2"/>
     </row>
@@ -6600,10 +6600,10 @@
         <v>131</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H18" s="2"/>
     </row>
@@ -6620,10 +6620,10 @@
         <v>140</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H19" s="2"/>
     </row>
@@ -6638,10 +6638,10 @@
         <v>142</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H20" s="2"/>
     </row>
@@ -6652,16 +6652,16 @@
         <v>44</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>362</v>
+        <v>341</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>157</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H21" s="2"/>
     </row>
@@ -6670,16 +6670,16 @@
       <c r="B22" s="2"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
-        <v>363</v>
+        <v>342</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>158</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H22" s="2"/>
     </row>
@@ -6690,16 +6690,16 @@
         <v>159</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>365</v>
+        <v>344</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H23" s="2"/>
     </row>
@@ -6714,10 +6714,10 @@
         <v>93</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H24" s="2"/>
     </row>
@@ -6734,10 +6734,10 @@
         <v>163</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H25" s="2"/>
     </row>
@@ -6754,10 +6754,10 @@
         <v>166</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H26" s="2"/>
     </row>
@@ -6772,10 +6772,10 @@
         <v>168</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H27" s="2"/>
     </row>
@@ -6792,10 +6792,10 @@
         <v>171</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H28" s="2"/>
     </row>
@@ -6812,10 +6812,10 @@
         <v>173</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H29" s="2"/>
     </row>
@@ -6830,10 +6830,10 @@
         <v>174</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H30" s="2"/>
     </row>
@@ -6841,7 +6841,7 @@
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="8" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>178</v>
@@ -6850,10 +6850,10 @@
         <v>179</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H31" s="2"/>
     </row>
@@ -6865,13 +6865,13 @@
         <v>180</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>368</v>
+        <v>347</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H32" s="2"/>
     </row>
@@ -6888,10 +6888,10 @@
         <v>148</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H33" s="2"/>
     </row>
@@ -6905,13 +6905,13 @@
         <v>145</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>309</v>
+        <v>291</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H34" s="2"/>
     </row>
@@ -6928,10 +6928,10 @@
         <v>149</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H35" s="2"/>
     </row>
@@ -6946,10 +6946,10 @@
         <v>151</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H36" s="2"/>
     </row>
@@ -6964,10 +6964,10 @@
         <v>153</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H37" s="2"/>
     </row>
@@ -6984,10 +6984,10 @@
         <v>156</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H38" s="2"/>
     </row>
@@ -6996,16 +6996,16 @@
       <c r="B39" s="2"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8" t="s">
-        <v>366</v>
+        <v>345</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>367</v>
+        <v>346</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H39" s="2"/>
     </row>
@@ -7022,10 +7022,10 @@
         <v>183</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H40" s="2"/>
     </row>
@@ -7042,10 +7042,10 @@
         <v>187</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H41" s="2"/>
     </row>
@@ -7060,14 +7060,14 @@
         <v>189</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H42" s="2"/>
     </row>
-    <row customHeight="1" ht="30" r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="31.5" r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="8" t="s">
@@ -7080,10 +7080,10 @@
         <v>192</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H43" s="2"/>
     </row>
@@ -7092,16 +7092,16 @@
       <c r="B44" s="2"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>193</v>
+        <v>348</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H44" s="2"/>
     </row>
@@ -7110,16 +7110,16 @@
       <c r="B45" s="2"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E45" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="E45" s="8" t="s">
-        <v>195</v>
-      </c>
       <c r="F45" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H45" s="2"/>
     </row>
@@ -7127,19 +7127,19 @@
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="E46" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="D46" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>197</v>
-      </c>
       <c r="F46" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H46" s="2"/>
     </row>
@@ -7148,16 +7148,16 @@
       <c r="B47" s="2"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H47" s="2"/>
     </row>
@@ -7165,128 +7165,132 @@
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D48" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="E48" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="E48" s="8" t="s">
-        <v>202</v>
-      </c>
       <c r="F48" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H48" s="2"/>
     </row>
-    <row customHeight="1" ht="30" r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="34.5" r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
-      <c r="C49" s="8" t="s">
-        <v>203</v>
-      </c>
+      <c r="C49" s="8"/>
       <c r="D49" s="8" t="s">
-        <v>204</v>
+        <v>362</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>205</v>
+        <v>363</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H49" s="2"/>
     </row>
-    <row customHeight="1" ht="57" r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
-      <c r="C50" s="8"/>
+      <c r="C50" s="8" t="s">
+        <v>202</v>
+      </c>
       <c r="D50" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H50" s="2"/>
     </row>
-    <row customHeight="1" ht="54" r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="57" r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="E51" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="E51" s="8" t="s">
-        <v>209</v>
-      </c>
       <c r="F51" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H51" s="2"/>
     </row>
-    <row customHeight="1" ht="30" r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="54" r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H52" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
-      <c r="C53" s="8" t="s">
-        <v>212</v>
-      </c>
+      <c r="C53" s="8"/>
       <c r="D53" s="8" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>320</v>
+        <v>210</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="H53" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
-      <c r="C54" s="8"/>
+      <c r="C54" s="8" t="s">
+        <v>211</v>
+      </c>
       <c r="D54" s="8" t="s">
-        <v>353</v>
+        <v>212</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
+        <v>301</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H54" s="2"/>
     </row>
     <row customHeight="1" ht="48" r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -7294,43 +7298,55 @@
       <c r="B55" s="2"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="E55" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="E55" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
+      <c r="F55" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H55" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="E56" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="E56" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
+      <c r="F56" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H56" s="2"/>
     </row>
-    <row customHeight="1" ht="30" r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="31.5" r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8" t="s">
-        <v>219</v>
+        <v>349</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
+        <v>350</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H57" s="2"/>
     </row>
     <row customHeight="1" ht="33" r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -7338,45 +7354,57 @@
       <c r="B58" s="2"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
+        <v>218</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H58" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D59" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="D59" s="8" t="s">
-        <v>225</v>
-      </c>
       <c r="E59" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
+        <v>220</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H59" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="E60" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="D60" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
+      <c r="F60" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H60" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -7384,304 +7412,378 @@
       <c r="B61" s="2"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
+        <v>226</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H61" s="2"/>
     </row>
     <row customHeight="1" ht="35.25" r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="8" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
+        <v>227</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H62" s="2"/>
     </row>
-    <row customHeight="1" ht="33" r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="33.75" r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
-      <c r="C63" s="8"/>
+      <c r="C63" s="8" t="s">
+        <v>358</v>
+      </c>
       <c r="D63" s="8" t="s">
-        <v>232</v>
+        <v>359</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
+        <v>360</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H63" s="2"/>
     </row>
-    <row customHeight="1" ht="30" r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="33" r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
-      <c r="C64" s="8" t="s">
-        <v>246</v>
-      </c>
+      <c r="C64" s="8"/>
       <c r="D64" s="8" t="s">
-        <v>235</v>
+        <v>351</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
+        <v>230</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H64" s="2"/>
     </row>
-    <row customHeight="1" ht="47.25" r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="33" r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="8" t="s">
-        <v>247</v>
+        <v>352</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>239</v>
+        <v>353</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
+        <v>354</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H65" s="2"/>
     </row>
-    <row customHeight="1" ht="30" r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="33" r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="8" t="s">
-        <v>248</v>
+        <v>355</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>238</v>
+        <v>356</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
+        <v>357</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H66" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
-      <c r="C67" s="8"/>
+      <c r="C67" s="8" t="s">
+        <v>241</v>
+      </c>
       <c r="D67" s="8" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
+        <v>232</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H67" s="2"/>
     </row>
-    <row customHeight="1" ht="38.25" r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="47.25" r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>243</v>
+        <v>361</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
+        <v>233</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H68" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
-      <c r="C69" s="8"/>
+      <c r="C69" s="8" t="s">
+        <v>243</v>
+      </c>
       <c r="D69" s="8" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
+        <v>235</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H69" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
-      <c r="C70" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="D70" s="10" t="s">
-        <v>252</v>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8" t="s">
+        <v>236</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
+        <v>237</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H70" s="2"/>
     </row>
-    <row customHeight="1" ht="30" r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="38.25" r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
-      <c r="C71" s="8"/>
+      <c r="C71" s="8" t="s">
+        <v>244</v>
+      </c>
       <c r="D71" s="8" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
+        <v>239</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H71" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
-      <c r="C72" s="8" t="s">
-        <v>254</v>
-      </c>
+      <c r="C72" s="8"/>
       <c r="D72" s="8" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="F72" s="2"/>
-      <c r="G72" s="2"/>
+        <v>249</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H72" s="2"/>
     </row>
-    <row customHeight="1" ht="65.25" r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>257</v>
+        <v>245</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>365</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>314</v>
-      </c>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
+        <v>295</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H73" s="2"/>
     </row>
-    <row customHeight="1" ht="53.25" r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="31.5" r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="8" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
+        <v>248</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H74" s="2"/>
     </row>
     <row customHeight="1" ht="30" r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="8" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>263</v>
+        <v>366</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="F75" s="2"/>
-      <c r="G75" s="2"/>
+        <v>296</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H75" s="2"/>
     </row>
-    <row customHeight="1" ht="30" r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="37.5" r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
-      <c r="C76" s="8"/>
+      <c r="C76" s="8" t="s">
+        <v>251</v>
+      </c>
       <c r="D76" s="8" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
+        <v>297</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H76" s="2"/>
     </row>
-    <row customHeight="1" ht="36" r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="40.5" r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="8" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
+        <v>255</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H77" s="2"/>
     </row>
-    <row customHeight="1" ht="37.5" r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="34.5" r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="8" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="F78" s="2"/>
-      <c r="G78" s="2"/>
+        <v>258</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="H78" s="2"/>
     </row>
-    <row customHeight="1" ht="40.5" r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
-      <c r="C79" s="8" t="s">
-        <v>271</v>
+      <c r="C79" s="11" t="s">
+        <v>298</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row customHeight="1" ht="34.5" r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
-      <c r="C80" s="8" t="s">
-        <v>274</v>
-      </c>
+      <c r="C80" s="8"/>
       <c r="D80" s="8" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
@@ -7690,14 +7792,12 @@
     <row customHeight="1" ht="30" r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
-      <c r="C81" s="11" t="s">
-        <v>317</v>
-      </c>
+      <c r="C81" s="8"/>
       <c r="D81" s="8" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
@@ -7708,24 +7808,24 @@
       <c r="B82" s="2"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row customHeight="1" ht="30" r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="49.5" r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
@@ -7736,24 +7836,24 @@
       <c r="B84" s="2"/>
       <c r="C84" s="8"/>
       <c r="D84" s="8" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>318</v>
+        <v>269</v>
       </c>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row customHeight="1" ht="49.5" r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="8"/>
       <c r="D85" s="8" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
@@ -7764,24 +7864,24 @@
       <c r="B86" s="2"/>
       <c r="C86" s="8"/>
       <c r="D86" s="8" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row customHeight="1" ht="30" r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row ht="60" r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="8"/>
       <c r="D87" s="8" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
@@ -7791,25 +7891,26 @@
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="8"/>
-      <c r="D88" s="8" t="s">
-        <v>283</v>
+      <c r="D88" s="3" t="s">
+        <v>273</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="F88" s="2"/>
+        <v>274</v>
+      </c>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row ht="75" r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="36" r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
-      <c r="C89" s="8"/>
+      <c r="C89" s="8" t="s">
+        <v>275</v>
+      </c>
       <c r="D89" s="8" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
@@ -7819,26 +7920,25 @@
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="8"/>
-      <c r="D90" s="3" t="s">
-        <v>291</v>
+      <c r="D90" s="8" t="s">
+        <v>280</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>292</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="F90" s="2"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row customHeight="1" ht="36" r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
-      <c r="C91" s="8" t="s">
-        <v>293</v>
-      </c>
+      <c r="C91" s="8"/>
       <c r="D91" s="8" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
@@ -7849,24 +7949,26 @@
       <c r="B92" s="2"/>
       <c r="C92" s="8"/>
       <c r="D92" s="8" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row customHeight="1" ht="30" r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="54" r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
-      <c r="C93" s="8"/>
+      <c r="C93" s="8" t="s">
+        <v>324</v>
+      </c>
       <c r="D93" s="8" t="s">
-        <v>299</v>
+        <v>364</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>300</v>
+        <v>325</v>
       </c>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
@@ -7877,70 +7979,70 @@
       <c r="B94" s="2"/>
       <c r="C94" s="8"/>
       <c r="D94" s="8" t="s">
-        <v>301</v>
+        <v>326</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>302</v>
+        <v>327</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row customHeight="1" ht="33" r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="32.25" r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
-      <c r="C95" s="8" t="s">
-        <v>343</v>
-      </c>
+      <c r="C95" s="8"/>
       <c r="D95" s="8" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row customHeight="1" ht="30" r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="33.75" r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
-      <c r="C96" s="8"/>
+      <c r="C96" s="8" t="s">
+        <v>285</v>
+      </c>
       <c r="D96" s="8" t="s">
-        <v>346</v>
+        <v>286</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>347</v>
+        <v>287</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row customHeight="1" ht="32.25" r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="8"/>
       <c r="D97" s="8" t="s">
-        <v>348</v>
+        <v>300</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>349</v>
+        <v>288</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row customHeight="1" ht="33.75" r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
-      <c r="C98" s="8" t="s">
+      <c r="C98" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="E98" s="8" t="s">
         <v>303</v>
-      </c>
-      <c r="D98" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="E98" s="8" t="s">
-        <v>305</v>
       </c>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
@@ -7948,164 +8050,154 @@
     </row>
     <row customHeight="1" ht="30" r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
-      <c r="B99" s="2"/>
+      <c r="B99" s="8" t="s">
+        <v>333</v>
+      </c>
       <c r="C99" s="8"/>
       <c r="D99" s="8" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row customHeight="1" ht="30" r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="44.25" r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="11" t="s">
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="E100" s="8" t="s">
         <v>307</v>
-      </c>
-      <c r="D100" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="E100" s="8" t="s">
-        <v>322</v>
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
     </row>
-    <row customHeight="1" ht="30" r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="45" r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="8" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="8" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
     </row>
-    <row customHeight="1" ht="44.25" r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="37.5" r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
-      <c r="B102" s="8"/>
+      <c r="B102" s="2"/>
       <c r="C102" s="8"/>
       <c r="D102" s="8" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
     </row>
-    <row customHeight="1" ht="36.75" r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="39" r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
-      <c r="B103" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="C103" s="8"/>
+      <c r="B103" s="2"/>
+      <c r="C103" s="8" t="s">
+        <v>308</v>
+      </c>
       <c r="D103" s="8" t="s">
-        <v>336</v>
+        <v>309</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>337</v>
+        <v>310</v>
       </c>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
     </row>
-    <row customHeight="1" ht="37.5" r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="34.5" r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="8"/>
       <c r="D104" s="8" t="s">
-        <v>338</v>
+        <v>311</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>339</v>
+        <v>312</v>
       </c>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
     </row>
-    <row customHeight="1" ht="39" r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
-      <c r="C105" s="8" t="s">
-        <v>327</v>
-      </c>
+      <c r="C105" s="8"/>
       <c r="D105" s="8" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="E105" s="8" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
     </row>
-    <row customHeight="1" ht="34.5" r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="50.25" r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="8"/>
       <c r="D106" s="8" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
     </row>
-    <row customHeight="1" ht="30" r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="35.25" r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
-      <c r="C107" s="8"/>
+      <c r="C107" s="8" t="s">
+        <v>321</v>
+      </c>
       <c r="D107" s="8" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="F107" s="2"/>
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
     </row>
-    <row customHeight="1" ht="50.25" r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="8"/>
-      <c r="D108" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E108" s="8" t="s">
-        <v>335</v>
-      </c>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
     </row>
-    <row customHeight="1" ht="35.25" r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
-      <c r="C109" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="D109" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="E109" s="8" t="s">
-        <v>342</v>
-      </c>
+      <c r="C109" s="8"/>
+      <c r="D109" s="8"/>
+      <c r="E109" s="8"/>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
@@ -9019,26 +9111,6 @@
       <c r="F200" s="2"/>
       <c r="G200" s="2"/>
       <c r="H200" s="2"/>
-    </row>
-    <row customHeight="1" ht="30" r="201" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A201" s="2"/>
-      <c r="B201" s="2"/>
-      <c r="C201" s="8"/>
-      <c r="D201" s="8"/>
-      <c r="E201" s="8"/>
-      <c r="F201" s="2"/>
-      <c r="G201" s="2"/>
-      <c r="H201" s="2"/>
-    </row>
-    <row customHeight="1" ht="30" r="202" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A202" s="2"/>
-      <c r="B202" s="2"/>
-      <c r="C202" s="8"/>
-      <c r="D202" s="8"/>
-      <c r="E202" s="8"/>
-      <c r="F202" s="2"/>
-      <c r="G202" s="2"/>
-      <c r="H202" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G20 G23:G1048576">
@@ -9058,6 +9130,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" verticalDpi="4294967295"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Driver updated to 73
</commit_message>
<xml_diff>
--- a/src/main/resources/WebStaff TC ExcelSheet/Automation Test test cases for WebStaff.xlsx
+++ b/src/main/resources/WebStaff TC ExcelSheet/Automation Test test cases for WebStaff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\QA\R&amp;DQA\Selenium\Chandra Workspace\WebStaff\src\main\resources\WebStaff TC ExcelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{13C15CAF-5935-40D8-A4ED-C6AAE633BA06}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
+  <xr:revisionPtr documentId="13_ncr:1_{2BF332B9-5FA6-4A6B-A99A-9CAF33E53ACF}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
   <bookViews>
     <workbookView windowHeight="7725" windowWidth="20400" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3762" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1743" uniqueCount="273">
   <si>
     <t>Step#</t>
   </si>
@@ -781,12 +781,6 @@
     <t>Add Attendee Group in ShowMan.</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>kulandasamyc</t>
-  </si>
-  <si>
     <t>System should and take to Search Page by default.</t>
   </si>
   <si>
@@ -920,7 +914,13 @@
     <t xml:space="preserve">System should show confirmation message as 'Confirmations will be sent to individuals with the send flag checkedSystem should remove the registrant Group and show blank values.' </t>
   </si>
   <si>
-    <t>Fail</t>
+    <t/>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>kulandasamyc</t>
   </si>
 </sst>
 </file>
@@ -1352,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C90" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,16 +1404,16 @@
         <v>17</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>237</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -1422,16 +1422,16 @@
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -1448,10 +1448,10 @@
         <v>228</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -1466,10 +1466,10 @@
         <v>38</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -1484,10 +1484,10 @@
         <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -1502,10 +1502,10 @@
         <v>21</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -1520,10 +1520,10 @@
         <v>23</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -1540,10 +1540,10 @@
         <v>25</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H9" s="2"/>
     </row>
@@ -1558,10 +1558,10 @@
         <v>27</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H10" s="2"/>
     </row>
@@ -1576,10 +1576,10 @@
         <v>29</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H11" s="2"/>
     </row>
@@ -1596,10 +1596,10 @@
         <v>40</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H12" s="2"/>
     </row>
@@ -1614,10 +1614,10 @@
         <v>42</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H13" s="2"/>
     </row>
@@ -1632,10 +1632,10 @@
         <v>43</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -1644,16 +1644,16 @@
       <c r="B15" s="2"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>188</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H15" s="2"/>
     </row>
@@ -1670,10 +1670,10 @@
         <v>188</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H16" s="2"/>
     </row>
@@ -1690,10 +1690,10 @@
         <v>33</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H17" s="2"/>
     </row>
@@ -1708,10 +1708,10 @@
         <v>35</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H18" s="2"/>
     </row>
@@ -1728,10 +1728,10 @@
         <v>44</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H19" s="2"/>
     </row>
@@ -1746,10 +1746,10 @@
         <v>46</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H20" s="2"/>
     </row>
@@ -1760,16 +1760,16 @@
         <v>9</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>61</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H21" s="2"/>
     </row>
@@ -1778,16 +1778,16 @@
       <c r="B22" s="2"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>62</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H22" s="2"/>
     </row>
@@ -1798,16 +1798,16 @@
         <v>63</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H23" s="2"/>
     </row>
@@ -1822,10 +1822,10 @@
         <v>16</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H24" s="2"/>
     </row>
@@ -1842,10 +1842,10 @@
         <v>67</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H25" s="2"/>
     </row>
@@ -1862,10 +1862,10 @@
         <v>70</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H26" s="2"/>
     </row>
@@ -1880,10 +1880,10 @@
         <v>72</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H27" s="2"/>
     </row>
@@ -1900,10 +1900,10 @@
         <v>75</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H28" s="2"/>
     </row>
@@ -1920,10 +1920,10 @@
         <v>77</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H29" s="2"/>
     </row>
@@ -1938,10 +1938,10 @@
         <v>78</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H30" s="2"/>
     </row>
@@ -1958,10 +1958,10 @@
         <v>83</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H31" s="2"/>
     </row>
@@ -1973,13 +1973,13 @@
         <v>84</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H32" s="2"/>
     </row>
@@ -1996,10 +1996,10 @@
         <v>52</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H33" s="2"/>
     </row>
@@ -2016,10 +2016,10 @@
         <v>189</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H34" s="2"/>
     </row>
@@ -2036,10 +2036,10 @@
         <v>53</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H35" s="2"/>
     </row>
@@ -2054,10 +2054,10 @@
         <v>55</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H36" s="2"/>
     </row>
@@ -2072,10 +2072,10 @@
         <v>57</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H37" s="2"/>
     </row>
@@ -2092,10 +2092,10 @@
         <v>60</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H38" s="2"/>
     </row>
@@ -2104,16 +2104,16 @@
       <c r="B39" s="2"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H39" s="2"/>
     </row>
@@ -2130,10 +2130,10 @@
         <v>87</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H40" s="2"/>
     </row>
@@ -2150,10 +2150,10 @@
         <v>91</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H41" s="2"/>
     </row>
@@ -2168,10 +2168,10 @@
         <v>93</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H42" s="2"/>
     </row>
@@ -2188,10 +2188,10 @@
         <v>96</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H43" s="2"/>
     </row>
@@ -2203,13 +2203,13 @@
         <v>190</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H44" s="2"/>
     </row>
@@ -2224,10 +2224,10 @@
         <v>98</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H45" s="2"/>
     </row>
@@ -2244,10 +2244,10 @@
         <v>100</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H46" s="2"/>
     </row>
@@ -2262,10 +2262,10 @@
         <v>101</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H47" s="2"/>
     </row>
@@ -2282,10 +2282,10 @@
         <v>105</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H48" s="2"/>
     </row>
@@ -2294,16 +2294,16 @@
       <c r="B49" s="2"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H49" s="2"/>
     </row>
@@ -2320,10 +2320,10 @@
         <v>108</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H50" s="2"/>
     </row>
@@ -2338,10 +2338,10 @@
         <v>111</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H51" s="2"/>
     </row>
@@ -2356,10 +2356,10 @@
         <v>112</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H52" s="2"/>
     </row>
@@ -2374,10 +2374,10 @@
         <v>114</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H53" s="2"/>
     </row>
@@ -2394,10 +2394,10 @@
         <v>198</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H54" s="2"/>
     </row>
@@ -2412,10 +2412,10 @@
         <v>118</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H55" s="2"/>
     </row>
@@ -2432,10 +2432,10 @@
         <v>121</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H56" s="2"/>
     </row>
@@ -2444,16 +2444,16 @@
       <c r="B57" s="2"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H57" s="2"/>
     </row>
@@ -2468,10 +2468,10 @@
         <v>122</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H58" s="2"/>
     </row>
@@ -2488,10 +2488,10 @@
         <v>124</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H59" s="2"/>
     </row>
@@ -2508,10 +2508,10 @@
         <v>128</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H60" s="2"/>
     </row>
@@ -2526,10 +2526,10 @@
         <v>130</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H61" s="2"/>
     </row>
@@ -2546,10 +2546,10 @@
         <v>131</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H62" s="2"/>
     </row>
@@ -2557,19 +2557,19 @@
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="E63" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="D63" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>257</v>
-      </c>
       <c r="F63" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H63" s="2"/>
     </row>
@@ -2578,16 +2578,16 @@
       <c r="B64" s="2"/>
       <c r="C64" s="6"/>
       <c r="D64" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>134</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H64" s="2"/>
     </row>
@@ -2595,19 +2595,19 @@
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="E65" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="D65" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>251</v>
-      </c>
       <c r="F65" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H65" s="2"/>
     </row>
@@ -2615,19 +2615,19 @@
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="E66" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="D66" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>254</v>
-      </c>
       <c r="F66" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H66" s="2"/>
     </row>
@@ -2644,10 +2644,10 @@
         <v>136</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H67" s="2"/>
     </row>
@@ -2658,16 +2658,16 @@
         <v>146</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>137</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H68" s="2"/>
     </row>
@@ -2684,10 +2684,10 @@
         <v>139</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H69" s="2"/>
     </row>
@@ -2702,10 +2702,10 @@
         <v>141</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H70" s="2"/>
     </row>
@@ -2722,10 +2722,10 @@
         <v>143</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H71" s="2"/>
     </row>
@@ -2740,10 +2740,10 @@
         <v>153</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H72" s="2"/>
     </row>
@@ -2754,16 +2754,16 @@
         <v>149</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>193</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H73" s="2"/>
     </row>
@@ -2780,10 +2780,10 @@
         <v>152</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H74" s="2"/>
     </row>
@@ -2794,16 +2794,16 @@
         <v>154</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>194</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H75" s="2"/>
     </row>
@@ -2820,10 +2820,10 @@
         <v>195</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H76" s="2"/>
     </row>
@@ -2840,10 +2840,10 @@
         <v>159</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H77" s="2"/>
     </row>
@@ -2860,10 +2860,10 @@
         <v>162</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H78" s="2"/>
     </row>
@@ -2880,10 +2880,10 @@
         <v>164</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H79" s="2"/>
     </row>
@@ -2898,10 +2898,10 @@
         <v>166</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H80" s="2"/>
     </row>
@@ -2916,10 +2916,10 @@
         <v>168</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H81" s="2"/>
     </row>
@@ -2934,10 +2934,10 @@
         <v>197</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H82" s="2"/>
     </row>
@@ -2949,13 +2949,13 @@
         <v>170</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H83" s="2"/>
     </row>
@@ -2967,13 +2967,13 @@
         <v>173</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H84" s="2"/>
     </row>
@@ -2988,10 +2988,10 @@
         <v>172</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H85" s="2"/>
     </row>
@@ -3000,16 +3000,16 @@
       <c r="B86" s="2"/>
       <c r="C86" s="6"/>
       <c r="D86" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>197</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H86" s="2"/>
     </row>
@@ -3018,16 +3018,16 @@
       <c r="B87" s="2"/>
       <c r="C87" s="6"/>
       <c r="D87" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H87" s="2"/>
     </row>
@@ -3044,10 +3044,10 @@
         <v>177</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H88" s="2"/>
     </row>
@@ -3062,10 +3062,10 @@
         <v>178</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H89" s="2"/>
     </row>
@@ -3080,10 +3080,10 @@
         <v>181</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H90" s="2"/>
     </row>
@@ -3098,10 +3098,10 @@
         <v>183</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H91" s="2"/>
     </row>
@@ -3112,16 +3112,16 @@
         <v>221</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E92" s="6" t="s">
         <v>222</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H92" s="2"/>
     </row>
@@ -3136,10 +3136,10 @@
         <v>224</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H93" s="2"/>
     </row>
@@ -3154,10 +3154,10 @@
         <v>226</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H94" s="2"/>
     </row>
@@ -3171,13 +3171,13 @@
         <v>185</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H95" s="2"/>
     </row>
@@ -3192,10 +3192,10 @@
         <v>186</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H96" s="2"/>
     </row>
@@ -3212,10 +3212,10 @@
         <v>200</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H97" s="2"/>
     </row>
@@ -3225,7 +3225,7 @@
         <v>230</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>201</v>
@@ -3234,10 +3234,10 @@
         <v>202</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H98" s="2"/>
     </row>
@@ -3252,10 +3252,10 @@
         <v>204</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H99" s="2"/>
     </row>
@@ -3265,7 +3265,7 @@
         <v>231</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>214</v>
@@ -3274,10 +3274,10 @@
         <v>215</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H100" s="2"/>
     </row>
@@ -3292,10 +3292,10 @@
         <v>217</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H101" s="2"/>
     </row>
@@ -3312,10 +3312,10 @@
         <v>207</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H102" s="2"/>
     </row>
@@ -3330,10 +3330,10 @@
         <v>209</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H103" s="2"/>
     </row>
@@ -3348,10 +3348,10 @@
         <v>211</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H104" s="2"/>
     </row>
@@ -3366,10 +3366,10 @@
         <v>213</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H105" s="2"/>
     </row>
@@ -3386,10 +3386,10 @@
         <v>220</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="H106" s="2"/>
     </row>

</xml_diff>